<commit_message>
removed dipendente --> docente
</commit_message>
<xml_diff>
--- a/ProgettazioneLogica.xlsx
+++ b/ProgettazioneLogica.xlsx
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:F88"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +846,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
add functions and fix
</commit_message>
<xml_diff>
--- a/ProgettazioneLogica.xlsx
+++ b/ProgettazioneLogica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTENTE\Documents\GitHub\UniversityExamSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E12929A-8FAE-4C1D-AF9F-A35D6AD25C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5238AF1-4C24-4297-B748-3A6BA06C9BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="96">
   <si>
     <t>Nome Tabella</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>char(6)</t>
   </si>
 </sst>
 </file>
@@ -674,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +915,7 @@
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -1226,7 +1229,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
@@ -1389,7 +1392,7 @@
         <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
@@ -1450,7 +1453,7 @@
         <v>46</v>
       </c>
       <c r="C70" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
@@ -1547,7 +1550,7 @@
         <v>46</v>
       </c>
       <c r="C79" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D79" t="s">
         <v>15</v>

</xml_diff>